<commit_message>
Averages now fill in to FOMC table.
</commit_message>
<xml_diff>
--- a/data/contracts.xlsx
+++ b/data/contracts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackkidney/Documents/fedwatch/fedtool/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF97590A-63B8-E540-A7CF-082BA1EB7341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF50BD7-27EC-AC4B-BB23-28EE5034287A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="500" windowWidth="27240" windowHeight="15260" xr2:uid="{FCCF7160-17C5-5F44-992D-D2DFBD308E97}"/>
   </bookViews>
@@ -150,8 +150,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -192,13 +193,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,7 +538,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -576,7 +578,7 @@
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="6">
         <v>94.67</v>
       </c>
       <c r="C2" s="5">
@@ -602,7 +604,7 @@
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="6">
         <v>94.674999999999997</v>
       </c>
       <c r="C3" s="5">
@@ -628,7 +630,7 @@
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="6">
         <v>94.685000000000002</v>
       </c>
       <c r="C4" s="5">
@@ -654,7 +656,7 @@
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="6">
         <v>94.74</v>
       </c>
       <c r="C5" s="5">
@@ -680,7 +682,7 @@
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="6">
         <v>94.795000000000002</v>
       </c>
       <c r="C6" s="5">
@@ -706,7 +708,7 @@
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="6">
         <v>94.87</v>
       </c>
       <c r="C7" s="5">
@@ -732,7 +734,7 @@
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="6">
         <v>94.935000000000002</v>
       </c>
       <c r="C8" s="5">
@@ -758,7 +760,7 @@
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="6">
         <v>95.02</v>
       </c>
       <c r="C9" s="5">
@@ -784,7 +786,7 @@
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="6">
         <v>95.105000000000004</v>
       </c>
       <c r="C10" s="5">
@@ -810,7 +812,7 @@
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="6">
         <v>95.2</v>
       </c>
       <c r="C11" s="5">
@@ -836,7 +838,7 @@
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="6">
         <v>95.254999999999995</v>
       </c>
       <c r="C12" s="5">
@@ -862,7 +864,7 @@
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="6">
         <v>95.334999999999994</v>
       </c>
       <c r="C13" s="5">
@@ -888,7 +890,7 @@
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="6">
         <v>95.43</v>
       </c>
       <c r="C14" s="5">
@@ -914,7 +916,7 @@
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="6">
         <v>95.51</v>
       </c>
       <c r="C15" s="5">
@@ -940,7 +942,7 @@
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="6">
         <v>95.594999999999999</v>
       </c>
       <c r="C16" s="5">
@@ -966,7 +968,7 @@
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="5">
@@ -992,7 +994,7 @@
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="5">
@@ -1018,7 +1020,7 @@
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="5">

</xml_diff>